<commit_message>
Changed --DTC to --DAT
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_QRS_TTS.xlsx
+++ b/curation/draft/collection/collection_specialization_QRS_TTS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cdisc-my.sharepoint.com/personal/dkottig_cdisc_org/Documents/01_BC/01_BC_Build/01_eCRF/QRS/TTS_LZZT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="215" documentId="13_ncr:1_{78DA25EC-0D12-4279-8ADF-D8AD59F6328D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88E3D2BD-F353-054E-9E8B-4815091AC5EB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56437DDB-565C-3C4C-ACDC-3599766CF077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="4140" windowWidth="29900" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="93">
   <si>
     <t>package_date</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>derivation_description</t>
+  </si>
+  <si>
+    <t>QSDAT</t>
   </si>
 </sst>
 </file>
@@ -433,10 +436,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -726,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y4" sqref="Y4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -963,10 +962,10 @@
         <v>41</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>45</v>
@@ -1387,7 +1386,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:36" ht="127">
+    <row r="10" spans="1:36" ht="160" customHeight="1">
       <c r="B10" s="5" t="s">
         <v>80</v>
       </c>

</xml_diff>

<commit_message>
DEC_ID for --DAT changed
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_QRS_TTS.xlsx
+++ b/curation/draft/collection/collection_specialization_QRS_TTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56437DDB-565C-3C4C-ACDC-3599766CF077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFC5140-A605-D449-8F89-B26CF4D75D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="4140" windowWidth="29900" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="94">
   <si>
     <t>package_date</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>QSDAT</t>
+  </si>
+  <si>
+    <t>C82515</t>
   </si>
 </sst>
 </file>
@@ -725,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -967,8 +970,8 @@
       <c r="N3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>45</v>
+      <c r="O3" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>66</v>

</xml_diff>